<commit_message>
completed article and enhanced code
</commit_message>
<xml_diff>
--- a/Excel Files/R Output/Results.xlsx
+++ b/Excel Files/R Output/Results.xlsx
@@ -490,7 +490,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Excel Files/Workpaper 2 Mistaken Filename.xlsx</t>
+          <t>Excel Files/Workpaper 3 Mistaken Filename.xlsx</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,7 +508,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Error: `path` does not exist: ‘Excel Files/Workpaper 2 Mistaken Filename.xlsx’
+          <t xml:space="preserve">Error: `path` does not exist: ‘Excel Files/Workpaper 3 Mistaken Filename.xlsx’
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
remove outline and finishing touches on article.
</commit_message>
<xml_diff>
--- a/Excel Files/R Output/Results.xlsx
+++ b/Excel Files/R Output/Results.xlsx
@@ -405,11 +405,6 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -430,11 +425,6 @@
       <c r="D3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -454,11 +444,6 @@
       </c>
       <c r="D4" t="b">
         <v>1</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
       </c>
     </row>
     <row r="5">

</xml_diff>